<commit_message>
update AZ for 6/6
</commit_message>
<xml_diff>
--- a/initial_claims/AZ/AZ_data.xlsx
+++ b/initial_claims/AZ/AZ_data.xlsx
@@ -1,40 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10607"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andy/Documents/GitHub/coronavirus-unemployment/states/AZ/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andy/Documents/GitHub/coronavirus-unemployment/initial_claims/AZ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7874B433-B5C9-664A-90A8-56F21DDE41FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{37960B25-25EF-9A4B-8203-FCF84DC469E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25360" windowHeight="14980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ClaimsbyAreaandDateTable " sheetId="1" r:id="rId1"/>
     <sheet name="OTWClaimsbyIndustryTable" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="51">
   <si>
     <t xml:space="preserve">NOTE: The data provided in these tables do no reflect the total number of initial UI claims filed within Arizona. The purpose of these data are to identify which industry sectors and geographic regions are recording the largest changes in initial unemployment insurance claims filings. For state-level total initial claims data, please visit the Arizona Office of Economic Opportunity's website at laborstats.az.gov. </t>
   </si>
@@ -114,7 +106,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Initial Unemployment Insurance Claims for Week Ending 5/30/20 by Area and Industry</t>
+    <t>Initial Unemployment Insurance Claims for Week Ending 6/6/20 by Area and Industry</t>
   </si>
   <si>
     <t>Industry</t>
@@ -186,7 +178,7 @@
     <t>Note: Unemployment insurance claims in this table do not represent area totals; Many unemployment claims were filed without an associated industry category.</t>
   </si>
   <si>
-    <t>Week-Over-Week Percent Change in Unemployment Insurance Claims for Week Ending 5/30/20</t>
+    <t>Week-Over-Week Percent Change in Unemployment Insurance Claims for Week Ending 6/6/20</t>
   </si>
 </sst>
 </file>
@@ -907,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U45"/>
+  <dimension ref="A1:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="134" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2013,1156 +2005,1274 @@
         <v>10301</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="34" t="s">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A22" s="10">
+        <v>43988</v>
+      </c>
+      <c r="B22" s="11">
+        <v>88</v>
+      </c>
+      <c r="C22" s="11">
+        <v>82</v>
+      </c>
+      <c r="D22" s="11">
+        <v>220</v>
+      </c>
+      <c r="E22" s="11">
+        <v>41</v>
+      </c>
+      <c r="F22" s="11">
+        <v>43</v>
+      </c>
+      <c r="G22" s="11">
+        <v>13</v>
+      </c>
+      <c r="H22" s="11">
+        <v>15</v>
+      </c>
+      <c r="I22" s="12">
+        <v>6809</v>
+      </c>
+      <c r="J22" s="12">
+        <v>172</v>
+      </c>
+      <c r="K22" s="12">
+        <v>155</v>
+      </c>
+      <c r="L22" s="12">
+        <v>1434</v>
+      </c>
+      <c r="M22" s="12">
+        <v>493</v>
+      </c>
+      <c r="N22" s="12">
+        <v>61</v>
+      </c>
+      <c r="O22" s="12">
+        <v>182</v>
+      </c>
+      <c r="P22" s="12">
+        <v>407</v>
+      </c>
+      <c r="Q22" s="12">
+        <v>75</v>
+      </c>
+      <c r="R22" s="12">
+        <v>41</v>
+      </c>
+      <c r="S22" s="12">
+        <v>10567</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A23" s="35" t="s">
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A24" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A26" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-    </row>
-    <row r="26" spans="1:19" s="3" customFormat="1" ht="43" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+    </row>
+    <row r="27" spans="1:19" s="3" customFormat="1" ht="43" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="K27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="L27" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M26" s="2" t="s">
+      <c r="M27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N26" s="2" t="s">
+      <c r="N27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O26" s="2" t="s">
+      <c r="O27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P26" s="2" t="s">
+      <c r="P27" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="2" t="s">
+      <c r="Q27" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R26" s="2" t="s">
+      <c r="R27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S26" s="2" t="s">
+      <c r="S27" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="15">
+    <row r="28" spans="1:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="15">
         <v>43869</v>
       </c>
-      <c r="B27" s="16">
+      <c r="B28" s="16">
         <v>0.25</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C28" s="16">
         <v>-0.42099999999999999</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D28" s="16">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="E27" s="16">
+      <c r="E28" s="16">
         <v>-0.44400000000000001</v>
       </c>
-      <c r="F27" s="16">
-        <v>0</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="H27" s="16">
+      <c r="F28" s="16">
+        <v>0</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="16">
         <v>-0.8</v>
       </c>
-      <c r="I27" s="16">
+      <c r="I28" s="16">
         <v>-7.0000000000000001E-3</v>
       </c>
-      <c r="J27" s="17">
+      <c r="J28" s="17">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="K27" s="17">
+      <c r="K28" s="17">
         <v>-7.4999999999999997E-2</v>
       </c>
-      <c r="L27" s="17">
+      <c r="L28" s="17">
         <v>-6.5000000000000002E-2</v>
       </c>
-      <c r="M27" s="17">
+      <c r="M28" s="17">
         <v>0.09</v>
       </c>
-      <c r="N27" s="17">
-        <v>0</v>
-      </c>
-      <c r="O27" s="17">
+      <c r="N28" s="17">
+        <v>0</v>
+      </c>
+      <c r="O28" s="17">
         <v>-9.0999999999999998E-2</v>
       </c>
-      <c r="P27" s="17">
+      <c r="P28" s="17">
         <v>-5.6000000000000001E-2</v>
       </c>
-      <c r="Q27" s="17">
-        <v>0</v>
-      </c>
-      <c r="R27" s="17">
-        <v>0</v>
-      </c>
-      <c r="S27" s="17">
+      <c r="Q28" s="17">
+        <v>0</v>
+      </c>
+      <c r="R28" s="17">
+        <v>0</v>
+      </c>
+      <c r="S28" s="17">
         <v>-2.7E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A28" s="18">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A29" s="18">
         <v>43876</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B29" s="19">
         <v>-0.2</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C29" s="19">
         <v>0.182</v>
       </c>
-      <c r="D28" s="19">
+      <c r="D29" s="19">
         <v>-0.44700000000000001</v>
       </c>
-      <c r="E28" s="19">
+      <c r="E29" s="19">
         <v>0.5</v>
       </c>
-      <c r="F28" s="19">
+      <c r="F29" s="19">
         <v>0.14299999999999999</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G29" s="19">
         <v>-1</v>
       </c>
-      <c r="H28" s="19">
-        <v>1</v>
-      </c>
-      <c r="I28" s="19">
+      <c r="H29" s="19">
+        <v>1</v>
+      </c>
+      <c r="I29" s="19">
         <v>-2.5999999999999999E-2</v>
       </c>
-      <c r="J28" s="20">
+      <c r="J29" s="20">
         <v>-6.3E-2</v>
       </c>
-      <c r="K28" s="20">
+      <c r="K29" s="20">
         <v>-8.1000000000000003E-2</v>
       </c>
-      <c r="L28" s="20">
+      <c r="L29" s="20">
         <v>-0.108</v>
       </c>
-      <c r="M28" s="20">
+      <c r="M29" s="20">
         <v>-0.11600000000000001</v>
       </c>
-      <c r="N28" s="20">
+      <c r="N29" s="20">
         <v>-0.308</v>
       </c>
-      <c r="O28" s="20">
+      <c r="O29" s="20">
         <v>-0.06</v>
       </c>
-      <c r="P28" s="20">
+      <c r="P29" s="20">
         <v>0.32400000000000001</v>
       </c>
-      <c r="Q28" s="20">
+      <c r="Q29" s="20">
         <v>-8.3000000000000004E-2</v>
       </c>
-      <c r="R28" s="20">
+      <c r="R29" s="20">
         <v>0.33300000000000002</v>
       </c>
-      <c r="S28" s="20">
+      <c r="S29" s="20">
         <v>-3.9E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A29" s="21">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A30" s="21">
         <v>43883</v>
       </c>
-      <c r="B29" s="22">
+      <c r="B30" s="22">
         <v>-6.3E-2</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C30" s="22">
         <v>-0.115</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D30" s="22">
         <v>0.115</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E30" s="22">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="F29" s="22">
+      <c r="F30" s="22">
         <v>0.875</v>
       </c>
-      <c r="G29" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="H29" s="22">
-        <v>1</v>
-      </c>
-      <c r="I29" s="22">
+      <c r="G30" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" s="22">
+        <v>1</v>
+      </c>
+      <c r="I30" s="22">
         <v>-0.159</v>
       </c>
-      <c r="J29" s="23">
+      <c r="J30" s="23">
         <v>0.156</v>
       </c>
-      <c r="K29" s="23">
+      <c r="K30" s="23">
         <v>-2.9000000000000001E-2</v>
       </c>
-      <c r="L29" s="23">
+      <c r="L30" s="23">
         <v>-2.1999999999999999E-2</v>
       </c>
-      <c r="M29" s="23">
+      <c r="M30" s="23">
         <v>-8.9999999999999993E-3</v>
       </c>
-      <c r="N29" s="23">
+      <c r="N30" s="23">
         <v>0.111</v>
       </c>
-      <c r="O29" s="23">
+      <c r="O30" s="23">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="P29" s="23">
+      <c r="P30" s="23">
         <v>-0.36699999999999999</v>
       </c>
-      <c r="Q29" s="23">
+      <c r="Q30" s="23">
         <v>-0.45500000000000002</v>
       </c>
-      <c r="R29" s="23">
+      <c r="R30" s="23">
         <v>-8.3000000000000004E-2</v>
       </c>
-      <c r="S29" s="23">
+      <c r="S30" s="23">
         <v>-0.11899999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A30" s="18">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A31" s="18">
         <v>43890</v>
       </c>
-      <c r="B30" s="19">
+      <c r="B31" s="19">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C31" s="19">
         <v>0.26100000000000001</v>
       </c>
-      <c r="D30" s="19">
+      <c r="D31" s="19">
         <v>-0.31</v>
       </c>
-      <c r="E30" s="19">
+      <c r="E31" s="19">
         <v>-0.125</v>
       </c>
-      <c r="F30" s="19">
+      <c r="F31" s="19">
         <v>-0.4</v>
       </c>
-      <c r="G30" s="19">
-        <v>1</v>
-      </c>
-      <c r="H30" s="19">
+      <c r="G31" s="19">
+        <v>1</v>
+      </c>
+      <c r="H31" s="19">
         <v>-0.5</v>
       </c>
-      <c r="I30" s="19">
+      <c r="I31" s="19">
         <v>-6.5000000000000002E-2</v>
       </c>
-      <c r="J30" s="20">
+      <c r="J31" s="20">
         <v>-0.192</v>
       </c>
-      <c r="K30" s="20">
+      <c r="K31" s="20">
         <v>-0.21199999999999999</v>
       </c>
-      <c r="L30" s="20">
+      <c r="L31" s="20">
         <v>-3.5000000000000003E-2</v>
       </c>
-      <c r="M30" s="20">
+      <c r="M31" s="20">
         <v>-9.4E-2</v>
       </c>
-      <c r="N30" s="20">
+      <c r="N31" s="20">
         <v>0.4</v>
       </c>
-      <c r="O30" s="20">
+      <c r="O31" s="20">
         <v>-0.06</v>
       </c>
-      <c r="P30" s="20">
+      <c r="P31" s="20">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="Q30" s="20">
+      <c r="Q31" s="20">
         <v>0.16700000000000001</v>
       </c>
-      <c r="R30" s="20">
+      <c r="R31" s="20">
         <v>0.36399999999999999</v>
       </c>
-      <c r="S30" s="20">
+      <c r="S31" s="20">
         <v>-5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A31" s="21">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A32" s="21">
         <v>43897</v>
       </c>
-      <c r="B31" s="22">
+      <c r="B32" s="22">
         <v>-0.188</v>
       </c>
-      <c r="C31" s="22">
+      <c r="C32" s="22">
         <v>-0.20699999999999999</v>
       </c>
-      <c r="D31" s="22">
-        <v>1</v>
-      </c>
-      <c r="E31" s="22">
+      <c r="D32" s="22">
+        <v>1</v>
+      </c>
+      <c r="E32" s="22">
         <v>-7.0999999999999994E-2</v>
       </c>
-      <c r="F31" s="22">
+      <c r="F32" s="22">
         <v>0.111</v>
       </c>
-      <c r="G31" s="22">
+      <c r="G32" s="22">
         <v>0.5</v>
       </c>
-      <c r="H31" s="22">
+      <c r="H32" s="22">
         <v>-0.25</v>
       </c>
-      <c r="I31" s="22">
+      <c r="I32" s="22">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="J31" s="23">
+      <c r="J32" s="23">
         <v>0.31</v>
       </c>
-      <c r="K31" s="23">
+      <c r="K32" s="23">
         <v>-0.26900000000000002</v>
       </c>
-      <c r="L31" s="23">
+      <c r="L32" s="23">
         <v>0.188</v>
       </c>
-      <c r="M31" s="23">
+      <c r="M32" s="23">
         <v>-0.17699999999999999</v>
       </c>
-      <c r="N31" s="23">
+      <c r="N32" s="23">
         <v>-0.14299999999999999</v>
       </c>
-      <c r="O31" s="23">
-        <v>0</v>
-      </c>
-      <c r="P31" s="23">
+      <c r="O32" s="23">
+        <v>0</v>
+      </c>
+      <c r="P32" s="23">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="Q31" s="23">
+      <c r="Q32" s="23">
         <v>0.85699999999999998</v>
       </c>
-      <c r="R31" s="23">
+      <c r="R32" s="23">
         <v>-0.53300000000000003</v>
       </c>
-      <c r="S31" s="23">
+      <c r="S32" s="23">
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A32" s="18">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A33" s="18">
         <v>43904</v>
       </c>
-      <c r="B32" s="19">
+      <c r="B33" s="19">
         <v>-0.154</v>
       </c>
-      <c r="C32" s="19">
+      <c r="C33" s="19">
         <v>0.34799999999999998</v>
       </c>
-      <c r="D32" s="19">
+      <c r="D33" s="19">
         <v>-0.05</v>
       </c>
-      <c r="E32" s="19">
+      <c r="E33" s="19">
         <v>-0.46200000000000002</v>
       </c>
-      <c r="F32" s="19">
+      <c r="F33" s="19">
         <v>-0.4</v>
       </c>
-      <c r="G32" s="19">
+      <c r="G33" s="19">
         <v>-0.33300000000000002</v>
       </c>
-      <c r="H32" s="19">
-        <v>1</v>
-      </c>
-      <c r="I32" s="19">
+      <c r="H33" s="19">
+        <v>1</v>
+      </c>
+      <c r="I33" s="19">
         <v>0.159</v>
       </c>
-      <c r="J32" s="20">
+      <c r="J33" s="20">
         <v>-0.109</v>
       </c>
-      <c r="K32" s="20">
+      <c r="K33" s="20">
         <v>0.52600000000000002</v>
       </c>
-      <c r="L32" s="20">
-        <v>0</v>
-      </c>
-      <c r="M32" s="20">
+      <c r="L33" s="20">
+        <v>0</v>
+      </c>
+      <c r="M33" s="20">
         <v>0.40500000000000003</v>
       </c>
-      <c r="N32" s="20">
+      <c r="N33" s="20">
         <v>-0.25</v>
       </c>
-      <c r="O32" s="20">
+      <c r="O33" s="20">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="P32" s="20">
+      <c r="P33" s="20">
         <v>0.51700000000000002</v>
       </c>
-      <c r="Q32" s="20">
+      <c r="Q33" s="20">
         <v>-0.23100000000000001</v>
       </c>
-      <c r="R32" s="20">
+      <c r="R33" s="20">
         <v>3.4289999999999998</v>
       </c>
-      <c r="S32" s="20">
+      <c r="S33" s="20">
         <v>0.14699999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A33" s="21">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A34" s="21">
         <v>43911</v>
       </c>
-      <c r="B33" s="22">
+      <c r="B34" s="22">
         <v>3</v>
       </c>
-      <c r="C33" s="22">
+      <c r="C34" s="22">
         <v>2.032</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D34" s="22">
         <v>14</v>
       </c>
-      <c r="E33" s="22">
+      <c r="E34" s="22">
         <v>3.1429999999999998</v>
       </c>
-      <c r="F33" s="22">
+      <c r="F34" s="22">
         <v>1.5</v>
       </c>
-      <c r="G33" s="22">
-        <v>1</v>
-      </c>
-      <c r="H33" s="22">
+      <c r="G34" s="22">
+        <v>1</v>
+      </c>
+      <c r="H34" s="22">
         <v>0.83299999999999996</v>
       </c>
-      <c r="I33" s="22">
+      <c r="I34" s="22">
         <v>9.5470000000000006</v>
       </c>
-      <c r="J33" s="23">
+      <c r="J34" s="23">
         <v>4.8979999999999997</v>
       </c>
-      <c r="K33" s="23">
+      <c r="K34" s="23">
         <v>3.2069999999999999</v>
       </c>
-      <c r="L33" s="23">
+      <c r="L34" s="23">
         <v>10.432</v>
       </c>
-      <c r="M33" s="23">
+      <c r="M34" s="23">
         <v>5.27</v>
       </c>
-      <c r="N33" s="23">
+      <c r="N34" s="23">
         <v>7.444</v>
       </c>
-      <c r="O33" s="23">
+      <c r="O34" s="23">
         <v>11.458</v>
       </c>
-      <c r="P33" s="23">
+      <c r="P34" s="23">
         <v>1.516</v>
       </c>
-      <c r="Q33" s="23">
+      <c r="Q34" s="23">
         <v>6.1</v>
       </c>
-      <c r="R33" s="23">
+      <c r="R34" s="23">
         <v>0.129</v>
       </c>
-      <c r="S33" s="23">
+      <c r="S34" s="23">
         <v>8.4830000000000005</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A34" s="18">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A35" s="18">
         <v>43918</v>
       </c>
-      <c r="B34" s="19">
+      <c r="B35" s="19">
         <v>2.5</v>
       </c>
-      <c r="C34" s="19">
+      <c r="C35" s="19">
         <v>3.883</v>
       </c>
-      <c r="D34" s="19">
+      <c r="D35" s="19">
         <v>1.982</v>
       </c>
-      <c r="E34" s="19">
+      <c r="E35" s="19">
         <v>4.6210000000000004</v>
       </c>
-      <c r="F34" s="19">
+      <c r="F35" s="19">
         <v>3.4670000000000001</v>
       </c>
-      <c r="G34" s="19">
+      <c r="G35" s="19">
         <v>3</v>
       </c>
-      <c r="H34" s="19">
+      <c r="H35" s="19">
         <v>2.1819999999999999</v>
       </c>
-      <c r="I34" s="19">
+      <c r="I35" s="19">
         <v>1.8080000000000001</v>
       </c>
-      <c r="J34" s="20">
+      <c r="J35" s="20">
         <v>3.54</v>
       </c>
-      <c r="K34" s="20">
+      <c r="K35" s="20">
         <v>2.2050000000000001</v>
       </c>
-      <c r="L34" s="20">
+      <c r="L35" s="20">
         <v>1.45</v>
       </c>
-      <c r="M34" s="20">
+      <c r="M35" s="20">
         <v>2.4660000000000002</v>
       </c>
-      <c r="N34" s="20">
+      <c r="N35" s="20">
         <v>2.3679999999999999</v>
       </c>
-      <c r="O34" s="20">
+      <c r="O35" s="20">
         <v>2.798</v>
       </c>
-      <c r="P34" s="20">
+      <c r="P35" s="20">
         <v>3.4409999999999998</v>
       </c>
-      <c r="Q34" s="20">
+      <c r="Q35" s="20">
         <v>2.056</v>
       </c>
-      <c r="R34" s="20">
+      <c r="R35" s="20">
         <v>1.6</v>
       </c>
-      <c r="S34" s="20">
+      <c r="S35" s="20">
         <v>1.879</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A35" s="21">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A36" s="21">
         <v>43925</v>
       </c>
-      <c r="B35" s="22">
+      <c r="B36" s="22">
         <v>0.247</v>
       </c>
-      <c r="C35" s="22">
+      <c r="C36" s="22">
         <v>0.32500000000000001</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D36" s="22">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="E35" s="22">
+      <c r="E36" s="22">
         <v>1.3560000000000001</v>
       </c>
-      <c r="F35" s="22">
+      <c r="F36" s="22">
         <v>1.284</v>
       </c>
-      <c r="G35" s="22">
+      <c r="G36" s="22">
         <v>6.3E-2</v>
       </c>
-      <c r="H35" s="22">
+      <c r="H36" s="22">
         <v>1.1140000000000001</v>
       </c>
-      <c r="I35" s="22">
+      <c r="I36" s="22">
         <v>0.28199999999999997</v>
       </c>
-      <c r="J35" s="23">
+      <c r="J36" s="23">
         <v>0.1</v>
       </c>
-      <c r="K35" s="23">
+      <c r="K36" s="23">
         <v>0.59299999999999997</v>
       </c>
-      <c r="L35" s="23">
+      <c r="L36" s="23">
         <v>0.40400000000000003</v>
       </c>
-      <c r="M35" s="23">
+      <c r="M36" s="23">
         <v>0.38600000000000001</v>
       </c>
-      <c r="N35" s="23">
+      <c r="N36" s="23">
         <v>0.42599999999999999</v>
       </c>
-      <c r="O35" s="23">
+      <c r="O36" s="23">
         <v>-5.1999999999999998E-2</v>
       </c>
-      <c r="P35" s="23">
+      <c r="P36" s="23">
         <v>0.5</v>
       </c>
-      <c r="Q35" s="23">
+      <c r="Q36" s="23">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="R35" s="23">
+      <c r="R36" s="23">
         <v>0.40699999999999997</v>
       </c>
-      <c r="S35" s="23">
+      <c r="S36" s="23">
         <v>0.28799999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A36" s="18">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A37" s="18">
         <v>43932</v>
       </c>
-      <c r="B36" s="19">
+      <c r="B37" s="19">
         <v>-0.20300000000000001</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C37" s="19">
         <v>-0.224</v>
       </c>
-      <c r="D36" s="19">
+      <c r="D37" s="19">
         <v>-0.377</v>
       </c>
-      <c r="E36" s="19">
+      <c r="E37" s="19">
         <v>-0.53900000000000003</v>
       </c>
-      <c r="F36" s="19">
+      <c r="F37" s="19">
         <v>-0.57499999999999996</v>
       </c>
-      <c r="G36" s="19">
+      <c r="G37" s="19">
         <v>-0.29399999999999998</v>
       </c>
-      <c r="H36" s="19">
+      <c r="H37" s="19">
         <v>-0.32400000000000001</v>
       </c>
-      <c r="I36" s="19">
+      <c r="I37" s="19">
         <v>-0.32700000000000001</v>
       </c>
-      <c r="J36" s="20">
+      <c r="J37" s="20">
         <v>-0.317</v>
       </c>
-      <c r="K36" s="20">
+      <c r="K37" s="20">
         <v>-0.27900000000000003</v>
       </c>
-      <c r="L36" s="20">
+      <c r="L37" s="20">
         <v>-0.33300000000000002</v>
       </c>
-      <c r="M36" s="20">
+      <c r="M37" s="20">
         <v>-0.33</v>
       </c>
-      <c r="N36" s="20">
+      <c r="N37" s="20">
         <v>-0.40500000000000003</v>
       </c>
-      <c r="O36" s="20">
+      <c r="O37" s="20">
         <v>-0.35099999999999998</v>
       </c>
-      <c r="P36" s="20">
+      <c r="P37" s="20">
         <v>0.214</v>
       </c>
-      <c r="Q36" s="20">
+      <c r="Q37" s="20">
         <v>-0.159</v>
       </c>
-      <c r="R36" s="20">
+      <c r="R37" s="20">
         <v>0.89100000000000001</v>
       </c>
-      <c r="S36" s="20">
+      <c r="S37" s="20">
         <v>-0.313</v>
       </c>
-      <c r="U36" t="s">
+      <c r="U37" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A37" s="21">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A38" s="21">
         <v>43939</v>
       </c>
-      <c r="B37" s="22">
+      <c r="B38" s="22">
         <v>-0.26800000000000002</v>
       </c>
-      <c r="C37" s="22">
+      <c r="C38" s="22">
         <v>-0.29399999999999998</v>
       </c>
-      <c r="D37" s="22">
+      <c r="D38" s="22">
         <v>-0.23799999999999999</v>
       </c>
-      <c r="E37" s="22">
+      <c r="E38" s="22">
         <v>-0.29899999999999999</v>
       </c>
-      <c r="F37" s="22">
+      <c r="F38" s="22">
         <v>-9.1999999999999998E-2</v>
       </c>
-      <c r="G37" s="22">
+      <c r="G38" s="22">
         <v>0.25</v>
       </c>
-      <c r="H37" s="22">
+      <c r="H38" s="22">
         <v>-0.46</v>
       </c>
-      <c r="I37" s="22">
+      <c r="I38" s="22">
         <v>-0.28399999999999997</v>
       </c>
-      <c r="J37" s="23">
+      <c r="J38" s="23">
         <v>-0.36099999999999999</v>
       </c>
-      <c r="K37" s="23">
+      <c r="K38" s="23">
         <v>-0.40799999999999997</v>
       </c>
-      <c r="L37" s="23">
+      <c r="L38" s="23">
         <v>-0.28399999999999997</v>
       </c>
-      <c r="M37" s="23">
+      <c r="M38" s="23">
         <v>-0.307</v>
       </c>
-      <c r="N37" s="23">
+      <c r="N38" s="23">
         <v>-0.27600000000000002</v>
       </c>
-      <c r="O37" s="23">
+      <c r="O38" s="23">
         <v>-0.26600000000000001</v>
       </c>
-      <c r="P37" s="23">
+      <c r="P38" s="23">
         <v>-0.161</v>
       </c>
-      <c r="Q37" s="23">
+      <c r="Q38" s="23">
         <v>-0.316</v>
       </c>
-      <c r="R37" s="23">
+      <c r="R38" s="23">
         <v>-0.19800000000000001</v>
       </c>
-      <c r="S37" s="23">
+      <c r="S38" s="23">
         <v>-0.28000000000000003</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A38" s="18">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A39" s="18">
         <v>43946</v>
       </c>
-      <c r="B38" s="19">
+      <c r="B39" s="19">
         <v>-0.08</v>
       </c>
-      <c r="C38" s="19">
+      <c r="C39" s="19">
         <v>-0.28799999999999998</v>
       </c>
-      <c r="D38" s="19">
+      <c r="D39" s="19">
         <v>-0.35899999999999999</v>
       </c>
-      <c r="E38" s="19">
+      <c r="E39" s="19">
         <v>-0.16900000000000001</v>
       </c>
-      <c r="F38" s="19">
+      <c r="F39" s="19">
         <v>-0.32200000000000001</v>
       </c>
-      <c r="G38" s="19">
+      <c r="G39" s="19">
         <v>-0.46700000000000003</v>
       </c>
-      <c r="H38" s="19">
+      <c r="H39" s="19">
         <v>-0.37</v>
       </c>
-      <c r="I38" s="19">
+      <c r="I39" s="19">
         <v>-0.31</v>
       </c>
-      <c r="J38" s="20">
+      <c r="J39" s="20">
         <v>-0.30299999999999999</v>
       </c>
-      <c r="K38" s="20">
+      <c r="K39" s="20">
         <v>-0.36099999999999999</v>
       </c>
-      <c r="L38" s="20">
+      <c r="L39" s="20">
         <v>-0.29199999999999998</v>
       </c>
-      <c r="M38" s="20">
+      <c r="M39" s="20">
         <v>-0.22700000000000001</v>
       </c>
-      <c r="N38" s="20">
+      <c r="N39" s="20">
         <v>-0.26800000000000002</v>
       </c>
-      <c r="O38" s="20">
+      <c r="O39" s="20">
         <v>-0.15</v>
       </c>
-      <c r="P38" s="20">
+      <c r="P39" s="20">
         <v>-0.17899999999999999</v>
       </c>
-      <c r="Q38" s="20">
+      <c r="Q39" s="20">
         <v>-0.20100000000000001</v>
       </c>
-      <c r="R38" s="20">
+      <c r="R39" s="20">
         <v>-8.2000000000000003E-2</v>
       </c>
-      <c r="S38" s="20">
+      <c r="S39" s="20">
         <v>-0.29099999999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A39" s="21">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A40" s="21">
         <v>43953</v>
       </c>
-      <c r="B39" s="22">
+      <c r="B40" s="22">
         <v>-0.40799999999999997</v>
       </c>
-      <c r="C39" s="22">
+      <c r="C40" s="22">
         <v>-0.19400000000000001</v>
       </c>
-      <c r="D39" s="22">
+      <c r="D40" s="22">
         <v>-0.25900000000000001</v>
       </c>
-      <c r="E39" s="22">
+      <c r="E40" s="22">
         <v>-0.13600000000000001</v>
       </c>
-      <c r="F39" s="22">
+      <c r="F40" s="22">
         <v>1.3</v>
       </c>
-      <c r="G39" s="22">
+      <c r="G40" s="22">
         <v>0.5</v>
       </c>
-      <c r="H39" s="22">
+      <c r="H40" s="22">
         <v>0.35299999999999998</v>
       </c>
-      <c r="I39" s="22">
+      <c r="I40" s="22">
         <v>-0.17899999999999999</v>
       </c>
-      <c r="J39" s="23">
+      <c r="J40" s="23">
         <v>-0.27800000000000002</v>
       </c>
-      <c r="K39" s="23">
+      <c r="K40" s="23">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="L39" s="23">
+      <c r="L40" s="23">
         <v>-0.25900000000000001</v>
       </c>
-      <c r="M39" s="23">
+      <c r="M40" s="23">
         <v>-0.13400000000000001</v>
       </c>
-      <c r="N39" s="23">
+      <c r="N40" s="23">
         <v>-0.16500000000000001</v>
       </c>
-      <c r="O39" s="23">
+      <c r="O40" s="23">
         <v>-0.47399999999999998</v>
       </c>
-      <c r="P39" s="23">
+      <c r="P40" s="23">
         <v>-0.32800000000000001</v>
       </c>
-      <c r="Q39" s="23">
+      <c r="Q40" s="23">
         <v>-0.26200000000000001</v>
       </c>
-      <c r="R39" s="23">
+      <c r="R40" s="23">
         <v>-0.46100000000000002</v>
       </c>
-      <c r="S39" s="23">
+      <c r="S40" s="23">
         <v>-0.20499999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A40" s="18">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A41" s="18">
         <v>43960</v>
       </c>
-      <c r="B40" s="19">
+      <c r="B41" s="19">
         <v>-0.16400000000000001</v>
       </c>
-      <c r="C40" s="19">
+      <c r="C41" s="19">
         <v>-0.33500000000000002</v>
       </c>
-      <c r="D40" s="19">
+      <c r="D41" s="19">
         <v>-0.24399999999999999</v>
       </c>
-      <c r="E40" s="19">
+      <c r="E41" s="19">
         <v>-0.38200000000000001</v>
       </c>
-      <c r="F40" s="19">
+      <c r="F41" s="19">
         <v>0.72799999999999998</v>
       </c>
-      <c r="G40" s="19">
+      <c r="G41" s="19">
         <v>0.83299999999999996</v>
       </c>
-      <c r="H40" s="19">
+      <c r="H41" s="19">
         <v>-0.217</v>
       </c>
-      <c r="I40" s="19">
+      <c r="I41" s="19">
         <v>-0.252</v>
       </c>
-      <c r="J40" s="20">
+      <c r="J41" s="20">
         <v>0.192</v>
       </c>
-      <c r="K40" s="20">
-        <v>0</v>
-      </c>
-      <c r="L40" s="20">
+      <c r="K41" s="20">
+        <v>0</v>
+      </c>
+      <c r="L41" s="20">
         <v>-0.19600000000000001</v>
       </c>
-      <c r="M40" s="20">
+      <c r="M41" s="20">
         <v>-0.29099999999999998</v>
       </c>
-      <c r="N40" s="20">
+      <c r="N41" s="20">
         <v>-3.1E-2</v>
       </c>
-      <c r="O40" s="20">
+      <c r="O41" s="20">
         <v>-0.39900000000000002</v>
       </c>
-      <c r="P40" s="20">
+      <c r="P41" s="20">
         <v>1.47</v>
       </c>
-      <c r="Q40" s="20">
+      <c r="Q41" s="20">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="R40" s="20">
+      <c r="R41" s="20">
         <v>-0.125</v>
       </c>
-      <c r="S40" s="20">
+      <c r="S41" s="20">
         <v>-0.156</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A41" s="21">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A42" s="21">
         <v>43967</v>
       </c>
-      <c r="B41" s="22">
+      <c r="B42" s="22">
         <v>0.29399999999999998</v>
       </c>
-      <c r="C41" s="22">
+      <c r="C42" s="22">
         <v>-0.10199999999999999</v>
       </c>
-      <c r="D41" s="22">
+      <c r="D42" s="22">
         <v>-8.5000000000000006E-2</v>
       </c>
-      <c r="E41" s="22">
+      <c r="E42" s="22">
         <v>-0.14499999999999999</v>
       </c>
-      <c r="F41" s="22">
+      <c r="F42" s="22">
         <v>-0.57899999999999996</v>
       </c>
-      <c r="G41" s="22">
+      <c r="G42" s="22">
         <v>0.72699999999999998</v>
       </c>
-      <c r="H41" s="22">
+      <c r="H42" s="22">
         <v>-0.5</v>
       </c>
-      <c r="I41" s="22">
+      <c r="I42" s="22">
         <v>-0.18</v>
       </c>
-      <c r="J41" s="23">
+      <c r="J42" s="23">
         <v>-0.58499999999999996</v>
       </c>
-      <c r="K41" s="23">
+      <c r="K42" s="23">
         <v>-0.26100000000000001</v>
       </c>
-      <c r="L41" s="23">
+      <c r="L42" s="23">
         <v>-0.22700000000000001</v>
       </c>
-      <c r="M41" s="23">
+      <c r="M42" s="23">
         <v>-5.6000000000000001E-2</v>
       </c>
-      <c r="N41" s="23">
+      <c r="N42" s="23">
         <v>-0.39800000000000002</v>
       </c>
-      <c r="O41" s="23">
+      <c r="O42" s="23">
         <v>-0.17799999999999999</v>
       </c>
-      <c r="P41" s="23">
+      <c r="P42" s="23">
         <v>-0.749</v>
       </c>
-      <c r="Q41" s="23">
+      <c r="Q42" s="23">
         <v>-0.26300000000000001</v>
       </c>
-      <c r="R41" s="23">
+      <c r="R42" s="23">
         <v>-0.42899999999999999</v>
       </c>
-      <c r="S41" s="23">
+      <c r="S42" s="23">
         <v>-0.26400000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A42" s="18">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A43" s="18">
         <v>43974</v>
       </c>
-      <c r="B42" s="19">
+      <c r="B43" s="19">
         <v>-0.152</v>
       </c>
-      <c r="C42" s="19">
+      <c r="C43" s="19">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="D42" s="19">
+      <c r="D43" s="19">
         <v>-8.8999999999999996E-2</v>
       </c>
-      <c r="E42" s="19">
+      <c r="E43" s="19">
         <v>0.27700000000000002</v>
       </c>
-      <c r="F42" s="19">
+      <c r="F43" s="19">
         <v>-0.06</v>
       </c>
-      <c r="G42" s="19">
+      <c r="G43" s="19">
         <v>-0.26300000000000001</v>
       </c>
-      <c r="H42" s="19">
+      <c r="H43" s="19">
         <v>0.55600000000000005</v>
       </c>
-      <c r="I42" s="19">
+      <c r="I43" s="19">
         <v>-8.2000000000000003E-2</v>
       </c>
-      <c r="J42" s="20">
+      <c r="J43" s="20">
         <v>0.13400000000000001</v>
       </c>
-      <c r="K42" s="20">
+      <c r="K43" s="20">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="L42" s="20">
+      <c r="L43" s="20">
         <v>1E-3</v>
       </c>
-      <c r="M42" s="20">
+      <c r="M43" s="20">
         <v>-0.126</v>
       </c>
-      <c r="N42" s="20">
+      <c r="N43" s="20">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="O42" s="20">
+      <c r="O43" s="20">
         <v>-0.18099999999999999</v>
       </c>
-      <c r="P42" s="20">
+      <c r="P43" s="20">
         <v>-0.18</v>
       </c>
-      <c r="Q42" s="20">
+      <c r="Q43" s="20">
         <v>-6.8000000000000005E-2</v>
       </c>
-      <c r="R42" s="20">
+      <c r="R43" s="20">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="S42" s="20">
+      <c r="S43" s="20">
         <v>-7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A43" s="21">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A44" s="21">
         <v>43981</v>
       </c>
-      <c r="B43" s="22">
+      <c r="B44" s="22">
         <v>1.179</v>
       </c>
-      <c r="C43" s="22">
+      <c r="C44" s="22">
         <v>-0.23499999999999999</v>
       </c>
-      <c r="D43" s="22">
+      <c r="D44" s="22">
         <v>0.10199999999999999</v>
       </c>
-      <c r="E43" s="22">
+      <c r="E44" s="22">
         <v>-0.25</v>
       </c>
-      <c r="F43" s="22">
+      <c r="F44" s="22">
         <v>-0.44400000000000001</v>
       </c>
-      <c r="G43" s="22">
+      <c r="G44" s="22">
         <v>-0.75</v>
       </c>
-      <c r="H43" s="22">
+      <c r="H44" s="22">
         <v>0.14299999999999999</v>
       </c>
-      <c r="I43" s="22">
+      <c r="I44" s="22">
         <v>-0.126</v>
       </c>
-      <c r="J43" s="23">
+      <c r="J44" s="23">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="K43" s="23">
+      <c r="K44" s="23">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="L43" s="23">
+      <c r="L44" s="23">
         <v>-0.153</v>
       </c>
-      <c r="M43" s="23">
+      <c r="M44" s="23">
         <v>-0.16800000000000001</v>
       </c>
-      <c r="N43" s="23">
+      <c r="N44" s="23">
         <v>0.17199999999999999</v>
       </c>
-      <c r="O43" s="23">
+      <c r="O44" s="23">
         <v>0.23699999999999999</v>
       </c>
-      <c r="P43" s="23">
+      <c r="P44" s="23">
         <v>-2.3E-2</v>
       </c>
-      <c r="Q43" s="23">
+      <c r="Q44" s="23">
         <v>0.109</v>
       </c>
-      <c r="R43" s="23">
+      <c r="R44" s="23">
         <v>-8.2000000000000003E-2</v>
       </c>
-      <c r="S43" s="23">
+      <c r="S44" s="23">
         <v>-0.108</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="37" t="s">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A45" s="18">
+        <v>43988</v>
+      </c>
+      <c r="B45" s="19">
+        <v>-0.27900000000000003</v>
+      </c>
+      <c r="C45" s="19">
+        <v>-9.9000000000000005E-2</v>
+      </c>
+      <c r="D45" s="19">
+        <v>-0.188</v>
+      </c>
+      <c r="E45" s="19">
+        <v>-8.8999999999999996E-2</v>
+      </c>
+      <c r="F45" s="19">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="G45" s="19">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="H45" s="19">
+        <v>-6.3E-2</v>
+      </c>
+      <c r="I45" s="19">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="J45" s="20">
+        <v>-0.104</v>
+      </c>
+      <c r="K45" s="20">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="L45" s="20">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="M45" s="20">
+        <v>-2.5999999999999999E-2</v>
+      </c>
+      <c r="N45" s="20">
+        <v>-0.10299999999999999</v>
+      </c>
+      <c r="O45" s="20">
+        <v>-0.20899999999999999</v>
+      </c>
+      <c r="P45" s="20">
+        <v>-4.4999999999999998E-2</v>
+      </c>
+      <c r="Q45" s="20">
+        <v>0.23</v>
+      </c>
+      <c r="R45" s="20">
+        <v>-8.8999999999999996E-2</v>
+      </c>
+      <c r="S45" s="20">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="37"/>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A45" s="31" t="s">
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A47" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="31"/>
+      <c r="B47" s="31"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A45:I45"/>
+    <mergeCell ref="A47:I47"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A22:I22"/>
     <mergeCell ref="A23:I23"/>
-    <mergeCell ref="A25:I25"/>
-    <mergeCell ref="A44:I44"/>
+    <mergeCell ref="A24:I24"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A46:I46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3173,8 +3283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3280,49 +3390,49 @@
         <v>7</v>
       </c>
       <c r="C5" s="26">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D5" s="26">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E5" s="26">
+        <v>6</v>
+      </c>
+      <c r="F5" s="26">
         <v>2</v>
       </c>
-      <c r="F5" s="26">
-        <v>4</v>
-      </c>
       <c r="G5" s="26">
         <v>0</v>
       </c>
       <c r="H5" s="26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I5" s="26">
-        <v>361</v>
+        <v>557</v>
       </c>
       <c r="J5" s="26">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="K5" s="26">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="L5" s="26">
-        <v>99</v>
+        <v>141</v>
       </c>
       <c r="M5" s="26">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="N5" s="26">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O5" s="26">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="P5" s="26">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="Q5" s="26">
-        <v>615</v>
+        <v>860</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -3330,52 +3440,52 @@
         <v>29</v>
       </c>
       <c r="B6" s="28">
+        <v>3</v>
+      </c>
+      <c r="C6" s="28">
+        <v>11</v>
+      </c>
+      <c r="D6" s="28">
+        <v>6</v>
+      </c>
+      <c r="E6" s="28">
+        <v>3</v>
+      </c>
+      <c r="F6" s="28">
+        <v>0</v>
+      </c>
+      <c r="G6" s="28">
+        <v>0</v>
+      </c>
+      <c r="H6" s="28">
+        <v>0</v>
+      </c>
+      <c r="I6" s="28">
+        <v>735</v>
+      </c>
+      <c r="J6" s="28">
+        <v>13</v>
+      </c>
+      <c r="K6" s="28">
+        <v>8</v>
+      </c>
+      <c r="L6" s="28">
+        <v>168</v>
+      </c>
+      <c r="M6" s="28">
+        <v>50</v>
+      </c>
+      <c r="N6" s="28">
         <v>2</v>
       </c>
-      <c r="C6" s="28">
-        <v>9</v>
-      </c>
-      <c r="D6" s="28">
-        <v>18</v>
-      </c>
-      <c r="E6" s="28">
-        <v>0</v>
-      </c>
-      <c r="F6" s="28">
-        <v>0</v>
-      </c>
-      <c r="G6" s="28">
-        <v>0</v>
-      </c>
-      <c r="H6" s="28">
-        <v>0</v>
-      </c>
-      <c r="I6" s="28">
-        <v>577</v>
-      </c>
-      <c r="J6" s="28">
-        <v>4</v>
-      </c>
-      <c r="K6" s="28">
-        <v>10</v>
-      </c>
-      <c r="L6" s="28">
-        <v>146</v>
-      </c>
-      <c r="M6" s="28">
-        <v>41</v>
-      </c>
-      <c r="N6" s="28">
-        <v>4</v>
-      </c>
       <c r="O6" s="28">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="P6" s="28">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="Q6" s="28">
-        <v>838</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -3386,7 +3496,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D7" s="26">
         <v>0</v>
@@ -3398,37 +3508,37 @@
         <v>1</v>
       </c>
       <c r="G7" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="26">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J7" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M7" s="26">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N7" s="26">
         <v>0</v>
       </c>
       <c r="O7" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P7" s="26">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="Q7" s="26">
-        <v>147</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -3436,16 +3546,16 @@
         <v>31</v>
       </c>
       <c r="B8" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="28">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E8" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="28">
         <v>0</v>
@@ -3454,34 +3564,34 @@
         <v>0</v>
       </c>
       <c r="H8" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="28">
-        <v>161</v>
+        <v>199</v>
       </c>
       <c r="J8" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="28">
+        <v>1</v>
+      </c>
+      <c r="L8" s="28">
+        <v>51</v>
+      </c>
+      <c r="M8" s="28">
+        <v>6</v>
+      </c>
+      <c r="N8" s="28">
+        <v>1</v>
+      </c>
+      <c r="O8" s="28">
         <v>2</v>
       </c>
-      <c r="L8" s="28">
-        <v>42</v>
-      </c>
-      <c r="M8" s="28">
-        <v>12</v>
-      </c>
-      <c r="N8" s="28">
-        <v>0</v>
-      </c>
-      <c r="O8" s="28">
-        <v>1</v>
-      </c>
       <c r="P8" s="28">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q8" s="28">
-        <v>236</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -3489,52 +3599,52 @@
         <v>32</v>
       </c>
       <c r="B9" s="26">
+        <v>10</v>
+      </c>
+      <c r="C9" s="26">
+        <v>4</v>
+      </c>
+      <c r="D9" s="26">
+        <v>18</v>
+      </c>
+      <c r="E9" s="26">
+        <v>3</v>
+      </c>
+      <c r="F9" s="26">
+        <v>14</v>
+      </c>
+      <c r="G9" s="26">
+        <v>6</v>
+      </c>
+      <c r="H9" s="26">
+        <v>1</v>
+      </c>
+      <c r="I9" s="26">
+        <v>479</v>
+      </c>
+      <c r="J9" s="26">
+        <v>12</v>
+      </c>
+      <c r="K9" s="26">
         <v>16</v>
       </c>
-      <c r="C9" s="26">
-        <v>12</v>
-      </c>
-      <c r="D9" s="26">
+      <c r="L9" s="26">
+        <v>102</v>
+      </c>
+      <c r="M9" s="26">
+        <v>36</v>
+      </c>
+      <c r="N9" s="26">
+        <v>2</v>
+      </c>
+      <c r="O9" s="26">
         <v>19</v>
       </c>
-      <c r="E9" s="26">
-        <v>2</v>
-      </c>
-      <c r="F9" s="26">
-        <v>8</v>
-      </c>
-      <c r="G9" s="26">
-        <v>1</v>
-      </c>
-      <c r="H9" s="26">
-        <v>0</v>
-      </c>
-      <c r="I9" s="26">
-        <v>343</v>
-      </c>
-      <c r="J9" s="26">
-        <v>10</v>
-      </c>
-      <c r="K9" s="26">
-        <v>15</v>
-      </c>
-      <c r="L9" s="26">
-        <v>73</v>
-      </c>
-      <c r="M9" s="26">
-        <v>48</v>
-      </c>
-      <c r="N9" s="26">
-        <v>4</v>
-      </c>
-      <c r="O9" s="26">
-        <v>12</v>
-      </c>
       <c r="P9" s="26">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="Q9" s="26">
-        <v>577</v>
+        <v>740</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -3542,19 +3652,19 @@
         <v>33</v>
       </c>
       <c r="B10" s="28">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C10" s="28">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" s="28">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="E10" s="28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10" s="28">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G10" s="28">
         <v>0</v>
@@ -3563,31 +3673,31 @@
         <v>1</v>
       </c>
       <c r="I10" s="28">
-        <v>592</v>
+        <v>532</v>
       </c>
       <c r="J10" s="28">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="K10" s="28">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="L10" s="28">
-        <v>192</v>
+        <v>153</v>
       </c>
       <c r="M10" s="28">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="N10" s="28">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="O10" s="28">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P10" s="28">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="Q10" s="28">
-        <v>1076</v>
+        <v>953</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -3598,10 +3708,10 @@
         <v>0</v>
       </c>
       <c r="C11" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="26">
         <v>0</v>
@@ -3616,31 +3726,31 @@
         <v>0</v>
       </c>
       <c r="I11" s="26">
-        <v>178</v>
+        <v>207</v>
       </c>
       <c r="J11" s="26">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K11" s="26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L11" s="26">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M11" s="26">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N11" s="26">
         <v>1</v>
       </c>
       <c r="O11" s="26">
+        <v>2</v>
+      </c>
+      <c r="P11" s="26">
         <v>4</v>
       </c>
-      <c r="P11" s="26">
-        <v>1</v>
-      </c>
       <c r="Q11" s="26">
-        <v>216</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -3648,16 +3758,16 @@
         <v>35</v>
       </c>
       <c r="B12" s="28">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C12" s="28">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D12" s="28">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E12" s="28">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" s="28">
         <v>1</v>
@@ -3666,34 +3776,34 @@
         <v>0</v>
       </c>
       <c r="H12" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="28">
-        <v>629</v>
+        <v>859</v>
       </c>
       <c r="J12" s="28">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="K12" s="28">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="L12" s="28">
-        <v>137</v>
+        <v>215</v>
       </c>
       <c r="M12" s="28">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="N12" s="28">
         <v>10</v>
       </c>
       <c r="O12" s="28">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="P12" s="28">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="Q12" s="28">
-        <v>1027</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -3701,13 +3811,13 @@
         <v>36</v>
       </c>
       <c r="B13" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="26">
         <v>0</v>
@@ -3719,10 +3829,10 @@
         <v>0</v>
       </c>
       <c r="H13" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="26">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="J13" s="26">
         <v>3</v>
@@ -3731,22 +3841,22 @@
         <v>0</v>
       </c>
       <c r="L13" s="26">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="M13" s="26">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N13" s="26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O13" s="26">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P13" s="26">
         <v>1</v>
       </c>
       <c r="Q13" s="26">
-        <v>110</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -3766,7 +3876,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="28">
         <v>0</v>
@@ -3775,19 +3885,19 @@
         <v>0</v>
       </c>
       <c r="I14" s="28">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="J14" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" s="28">
         <v>0</v>
       </c>
       <c r="L14" s="28">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M14" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N14" s="28">
         <v>0</v>
@@ -3796,10 +3906,10 @@
         <v>1</v>
       </c>
       <c r="P14" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="28">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -3810,49 +3920,49 @@
         <v>0</v>
       </c>
       <c r="C15" s="26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="26">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E15" s="26">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F15" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="26">
         <v>0</v>
       </c>
       <c r="I15" s="26">
-        <v>481</v>
+        <v>622</v>
       </c>
       <c r="J15" s="26">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="K15" s="26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L15" s="26">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="M15" s="26">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="N15" s="26">
         <v>0</v>
       </c>
       <c r="O15" s="26">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P15" s="26">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Q15" s="26">
-        <v>624</v>
+        <v>788</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
@@ -3860,40 +3970,40 @@
         <v>39</v>
       </c>
       <c r="B16" s="28">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C16" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="28">
         <v>0</v>
       </c>
       <c r="E16" s="28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F16" s="28">
         <v>4</v>
       </c>
       <c r="G16" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="28">
         <v>0</v>
       </c>
       <c r="I16" s="28">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J16" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="28">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="M16" s="28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N16" s="28">
         <v>0</v>
@@ -3905,7 +4015,7 @@
         <v>0</v>
       </c>
       <c r="Q16" s="28">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
@@ -3916,25 +4026,25 @@
         <v>2</v>
       </c>
       <c r="C17" s="26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D17" s="26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17" s="26">
         <v>1</v>
       </c>
       <c r="F17" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="26">
         <v>0</v>
       </c>
       <c r="H17" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="26">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="J17" s="26">
         <v>1</v>
@@ -3943,22 +4053,22 @@
         <v>2</v>
       </c>
       <c r="L17" s="26">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="M17" s="26">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="N17" s="26">
         <v>0</v>
       </c>
       <c r="O17" s="26">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P17" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q17" s="26">
-        <v>174</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
@@ -3969,49 +4079,49 @@
         <v>1</v>
       </c>
       <c r="C18" s="28">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D18" s="28">
+        <v>8</v>
+      </c>
+      <c r="E18" s="28">
+        <v>4</v>
+      </c>
+      <c r="F18" s="28">
+        <v>1</v>
+      </c>
+      <c r="G18" s="28">
+        <v>0</v>
+      </c>
+      <c r="H18" s="28">
+        <v>1</v>
+      </c>
+      <c r="I18" s="28">
+        <v>282</v>
+      </c>
+      <c r="J18" s="28">
+        <v>2</v>
+      </c>
+      <c r="K18" s="28">
+        <v>0</v>
+      </c>
+      <c r="L18" s="28">
+        <v>53</v>
+      </c>
+      <c r="M18" s="28">
+        <v>20</v>
+      </c>
+      <c r="N18" s="28">
         <v>7</v>
       </c>
-      <c r="E18" s="28">
-        <v>1</v>
-      </c>
-      <c r="F18" s="28">
-        <v>1</v>
-      </c>
-      <c r="G18" s="28">
-        <v>0</v>
-      </c>
-      <c r="H18" s="28">
-        <v>1</v>
-      </c>
-      <c r="I18" s="28">
-        <v>253</v>
-      </c>
-      <c r="J18" s="28">
-        <v>1</v>
-      </c>
-      <c r="K18" s="28">
-        <v>3</v>
-      </c>
-      <c r="L18" s="28">
-        <v>40</v>
-      </c>
-      <c r="M18" s="28">
+      <c r="O18" s="28">
         <v>14</v>
-      </c>
-      <c r="N18" s="28">
-        <v>1</v>
-      </c>
-      <c r="O18" s="28">
-        <v>1</v>
       </c>
       <c r="P18" s="28">
         <v>7</v>
       </c>
       <c r="Q18" s="28">
-        <v>336</v>
+        <v>408</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
@@ -4019,52 +4129,52 @@
         <v>42</v>
       </c>
       <c r="B19" s="26">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C19" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="26">
+        <v>10</v>
+      </c>
+      <c r="E19" s="26">
+        <v>5</v>
+      </c>
+      <c r="F19" s="26">
+        <v>1</v>
+      </c>
+      <c r="G19" s="26">
+        <v>0</v>
+      </c>
+      <c r="H19" s="26">
+        <v>2</v>
+      </c>
+      <c r="I19" s="26">
+        <v>75</v>
+      </c>
+      <c r="J19" s="26">
+        <v>3</v>
+      </c>
+      <c r="K19" s="26">
+        <v>15</v>
+      </c>
+      <c r="L19" s="26">
+        <v>17</v>
+      </c>
+      <c r="M19" s="26">
+        <v>6</v>
+      </c>
+      <c r="N19" s="26">
+        <v>1</v>
+      </c>
+      <c r="O19" s="26">
         <v>4</v>
       </c>
-      <c r="E19" s="26">
-        <v>6</v>
-      </c>
-      <c r="F19" s="26">
-        <v>1</v>
-      </c>
-      <c r="G19" s="26">
-        <v>0</v>
-      </c>
-      <c r="H19" s="26">
-        <v>1</v>
-      </c>
-      <c r="I19" s="26">
-        <v>53</v>
-      </c>
-      <c r="J19" s="26">
-        <v>2</v>
-      </c>
-      <c r="K19" s="26">
-        <v>14</v>
-      </c>
-      <c r="L19" s="26">
-        <v>9</v>
-      </c>
-      <c r="M19" s="26">
-        <v>9</v>
-      </c>
-      <c r="N19" s="26">
-        <v>0</v>
-      </c>
-      <c r="O19" s="26">
+      <c r="P19" s="26">
         <v>5</v>
       </c>
-      <c r="P19" s="26">
-        <v>3</v>
-      </c>
       <c r="Q19" s="26">
-        <v>118</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
@@ -4075,10 +4185,10 @@
         <v>0</v>
       </c>
       <c r="C20" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E20" s="28">
         <v>0</v>
@@ -4093,31 +4203,31 @@
         <v>0</v>
       </c>
       <c r="I20" s="28">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="J20" s="28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K20" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L20" s="28">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="M20" s="28">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="N20" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O20" s="28">
         <v>4</v>
       </c>
       <c r="P20" s="28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q20" s="28">
-        <v>118</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
@@ -4125,40 +4235,40 @@
         <v>44</v>
       </c>
       <c r="B21" s="26">
+        <v>2</v>
+      </c>
+      <c r="C21" s="26">
         <v>4</v>
       </c>
-      <c r="C21" s="26">
+      <c r="D21" s="26">
+        <v>18</v>
+      </c>
+      <c r="E21" s="26">
         <v>5</v>
       </c>
-      <c r="D21" s="26">
-        <v>13</v>
-      </c>
-      <c r="E21" s="26">
+      <c r="F21" s="26">
+        <v>7</v>
+      </c>
+      <c r="G21" s="26">
+        <v>0</v>
+      </c>
+      <c r="H21" s="26">
         <v>3</v>
       </c>
-      <c r="F21" s="26">
-        <v>1</v>
-      </c>
-      <c r="G21" s="26">
-        <v>0</v>
-      </c>
-      <c r="H21" s="26">
-        <v>0</v>
-      </c>
       <c r="I21" s="26">
-        <v>476</v>
+        <v>546</v>
       </c>
       <c r="J21" s="26">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="K21" s="26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L21" s="26">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="M21" s="26">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N21" s="26">
         <v>5</v>
@@ -4167,10 +4277,10 @@
         <v>12</v>
       </c>
       <c r="P21" s="26">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="Q21" s="26">
-        <v>687</v>
+        <v>808</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
@@ -4184,46 +4294,46 @@
         <v>3</v>
       </c>
       <c r="D22" s="28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E22" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" s="28">
         <v>1</v>
       </c>
       <c r="H22" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I22" s="28">
-        <v>213</v>
+        <v>277</v>
       </c>
       <c r="J22" s="28">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K22" s="28">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L22" s="28">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="M22" s="28">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="N22" s="28">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="O22" s="28">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="P22" s="28">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q22" s="28">
-        <v>299</v>
+        <v>391</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
@@ -4234,7 +4344,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="26">
         <v>0</v>
@@ -4246,25 +4356,25 @@
         <v>1</v>
       </c>
       <c r="G23" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="26">
         <v>0</v>
       </c>
       <c r="I23" s="26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J23" s="26">
         <v>0</v>
       </c>
       <c r="K23" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23" s="26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M23" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23" s="26">
         <v>0</v>
@@ -4273,10 +4383,10 @@
         <v>0</v>
       </c>
       <c r="P23" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q23" s="26">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
@@ -4284,10 +4394,10 @@
         <v>47</v>
       </c>
       <c r="B24" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="28">
         <v>3</v>
@@ -4296,40 +4406,40 @@
         <v>0</v>
       </c>
       <c r="F24" s="28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G24" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" s="28">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="J24" s="28">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K24" s="28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L24" s="28">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="M24" s="28">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="N24" s="28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O24" s="28">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P24" s="28">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="Q24" s="28">
-        <v>278</v>
+        <v>310</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
@@ -4337,52 +4447,52 @@
         <v>18</v>
       </c>
       <c r="B25" s="26">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C25" s="26">
+        <v>9</v>
+      </c>
+      <c r="D25" s="26">
+        <v>15</v>
+      </c>
+      <c r="E25" s="26">
+        <v>3</v>
+      </c>
+      <c r="F25" s="26">
+        <v>2</v>
+      </c>
+      <c r="G25" s="26">
+        <v>4</v>
+      </c>
+      <c r="H25" s="26">
+        <v>2</v>
+      </c>
+      <c r="I25" s="26">
+        <v>747</v>
+      </c>
+      <c r="J25" s="26">
         <v>19</v>
       </c>
-      <c r="D25" s="26">
-        <v>48</v>
-      </c>
-      <c r="E25" s="26">
-        <v>9</v>
-      </c>
-      <c r="F25" s="26">
-        <v>8</v>
-      </c>
-      <c r="G25" s="26">
-        <v>2</v>
-      </c>
-      <c r="H25" s="26">
-        <v>3</v>
-      </c>
-      <c r="I25" s="26">
-        <v>1555</v>
-      </c>
-      <c r="J25" s="26">
-        <v>36</v>
-      </c>
       <c r="K25" s="26">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="L25" s="26">
-        <v>343</v>
+        <v>129</v>
       </c>
       <c r="M25" s="26">
-        <v>134</v>
+        <v>65</v>
       </c>
       <c r="N25" s="26">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="O25" s="26">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="P25" s="26">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="Q25" s="26">
-        <v>2378</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
@@ -4390,13 +4500,13 @@
         <v>48</v>
       </c>
       <c r="B26" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" s="28">
         <v>0</v>
       </c>
       <c r="D26" s="28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E26" s="28">
         <v>0</v>
@@ -4411,7 +4521,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="28">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="J26" s="28">
         <v>0</v>
@@ -4420,7 +4530,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M26" s="28">
         <v>0</v>
@@ -4432,10 +4542,10 @@
         <v>0</v>
       </c>
       <c r="P26" s="28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q26" s="28">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
@@ -4563,73 +4673,73 @@
       <c r="A33" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="29">
-        <v>0.75</v>
+      <c r="B33" s="29" t="s">
+        <v>24</v>
       </c>
       <c r="C33" s="29">
-        <v>-0.3</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="D33" s="29">
-        <v>-0.49099999999999999</v>
+        <v>0.44400000000000001</v>
       </c>
       <c r="E33" s="29">
-        <v>-0.33300000000000002</v>
+        <v>2</v>
       </c>
       <c r="F33" s="29">
+        <v>-0.5</v>
+      </c>
+      <c r="G33" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" s="29">
+        <v>-1</v>
+      </c>
+      <c r="I33" s="29">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="J33" s="29">
+        <v>-0.375</v>
+      </c>
+      <c r="K33" s="29">
         <v>0.33300000000000002</v>
       </c>
-      <c r="G33" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="H33" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I33" s="29">
-        <v>-0.20499999999999999</v>
-      </c>
-      <c r="J33" s="29">
-        <v>-0.2</v>
-      </c>
-      <c r="K33" s="29">
-        <v>0.5</v>
-      </c>
       <c r="L33" s="29">
-        <v>-0.161</v>
+        <v>0.42399999999999999</v>
       </c>
       <c r="M33" s="29">
-        <v>-0.378</v>
+        <v>0.32100000000000001</v>
       </c>
       <c r="N33" s="29">
-        <v>1</v>
+        <v>-0.375</v>
       </c>
       <c r="O33" s="29">
-        <v>9.0999999999999998E-2</v>
+        <v>-0.375</v>
       </c>
       <c r="P33" s="29">
-        <v>0.313</v>
+        <v>-0.14299999999999999</v>
       </c>
       <c r="Q33" s="29">
-        <v>-0.191</v>
+        <v>0.39800000000000002</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="30" t="s">
-        <v>24</v>
+      <c r="B34" s="30">
+        <v>0.5</v>
       </c>
       <c r="C34" s="30">
-        <v>0.28599999999999998</v>
+        <v>0.222</v>
       </c>
       <c r="D34" s="30">
-        <v>1</v>
-      </c>
-      <c r="E34" s="30">
-        <v>-1</v>
-      </c>
-      <c r="F34" s="30">
-        <v>-1</v>
+        <v>-0.66700000000000004</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="30" t="s">
+        <v>24</v>
       </c>
       <c r="G34" s="30" t="s">
         <v>24</v>
@@ -4638,31 +4748,31 @@
         <v>24</v>
       </c>
       <c r="I34" s="30">
-        <v>0.03</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="J34" s="30">
+        <v>2.25</v>
+      </c>
+      <c r="K34" s="30">
         <v>-0.2</v>
       </c>
-      <c r="K34" s="30">
-        <v>2.3330000000000002</v>
-      </c>
       <c r="L34" s="30">
-        <v>0.41699999999999998</v>
+        <v>0.151</v>
       </c>
       <c r="M34" s="30">
-        <v>-8.8999999999999996E-2</v>
+        <v>0.22</v>
       </c>
       <c r="N34" s="30">
+        <v>-0.5</v>
+      </c>
+      <c r="O34" s="30">
         <v>0.33300000000000002</v>
       </c>
-      <c r="O34" s="30">
-        <v>0.28599999999999998</v>
-      </c>
       <c r="P34" s="30">
-        <v>-0.308</v>
+        <v>0.44400000000000001</v>
       </c>
       <c r="Q34" s="30">
-        <v>8.6999999999999994E-2</v>
+        <v>0.23699999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
@@ -4673,7 +4783,7 @@
         <v>24</v>
       </c>
       <c r="C35" s="29">
-        <v>-0.33300000000000002</v>
+        <v>1</v>
       </c>
       <c r="D35" s="29" t="s">
         <v>24</v>
@@ -4688,34 +4798,34 @@
         <v>24</v>
       </c>
       <c r="H35" s="29">
-        <v>1</v>
-      </c>
-      <c r="I35" s="29" t="s">
-        <v>24</v>
+        <v>-0.5</v>
+      </c>
+      <c r="I35" s="29">
+        <v>0.16700000000000001</v>
       </c>
       <c r="J35" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="K35" s="29">
-        <v>-1</v>
-      </c>
-      <c r="L35" s="29" t="s">
-        <v>24</v>
+      <c r="K35" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="L35" s="29">
+        <v>1</v>
       </c>
       <c r="M35" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="N35" s="29">
-        <v>-1</v>
-      </c>
-      <c r="O35" s="29" t="s">
-        <v>24</v>
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="N35" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="O35" s="29">
+        <v>-0.5</v>
       </c>
       <c r="P35" s="29">
-        <v>-0.158</v>
+        <v>-0.27600000000000002</v>
       </c>
       <c r="Q35" s="29">
-        <v>-0.13</v>
+        <v>-0.17</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
@@ -4725,50 +4835,50 @@
       <c r="B36" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="30">
+      <c r="C36" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="30">
+        <v>-0.375</v>
+      </c>
+      <c r="E36" s="30">
+        <v>1</v>
+      </c>
+      <c r="F36" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G36" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" s="30">
         <v>-1</v>
       </c>
-      <c r="D36" s="30">
-        <v>0.6</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="F36" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="G36" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="H36" s="30">
+      <c r="I36" s="30">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="J36" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="K36" s="30">
         <v>-0.5</v>
       </c>
-      <c r="I36" s="30">
-        <v>-0.439</v>
-      </c>
-      <c r="J36" s="30">
-        <v>-1</v>
-      </c>
-      <c r="K36" s="30">
-        <v>1</v>
-      </c>
       <c r="L36" s="30">
-        <v>-0.55300000000000005</v>
+        <v>0.214</v>
       </c>
       <c r="M36" s="30">
-        <v>-0.36799999999999999</v>
-      </c>
-      <c r="N36" s="30">
-        <v>-1</v>
-      </c>
-      <c r="O36" s="30" t="s">
-        <v>24</v>
+        <v>-0.5</v>
+      </c>
+      <c r="N36" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="O36" s="30">
+        <v>1</v>
       </c>
       <c r="P36" s="30">
-        <v>-0.2</v>
+        <v>-0.125</v>
       </c>
       <c r="Q36" s="30">
-        <v>-0.443</v>
+        <v>0.17399999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
@@ -4776,52 +4886,52 @@
         <v>32</v>
       </c>
       <c r="B37" s="29">
-        <v>1.286</v>
+        <v>-0.375</v>
       </c>
       <c r="C37" s="29">
+        <v>-0.66700000000000004</v>
+      </c>
+      <c r="D37" s="29">
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="E37" s="29">
         <v>0.5</v>
       </c>
-      <c r="D37" s="29">
-        <v>0.35699999999999998</v>
-      </c>
-      <c r="E37" s="29">
-        <v>-0.33300000000000002</v>
-      </c>
-      <c r="F37" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="G37" s="29" t="s">
-        <v>24</v>
+      <c r="F37" s="29">
+        <v>0.75</v>
+      </c>
+      <c r="G37" s="29">
+        <v>5</v>
       </c>
       <c r="H37" s="29" t="s">
         <v>24</v>
       </c>
       <c r="I37" s="29">
-        <v>-2.3E-2</v>
+        <v>0.39700000000000002</v>
       </c>
       <c r="J37" s="29">
-        <v>-0.16700000000000001</v>
-      </c>
-      <c r="K37" s="29" t="s">
-        <v>24</v>
+        <v>0.2</v>
+      </c>
+      <c r="K37" s="29">
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="L37" s="29">
-        <v>-1.4E-2</v>
+        <v>0.39700000000000002</v>
       </c>
       <c r="M37" s="29">
-        <v>0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="N37" s="29">
-        <v>3</v>
+        <v>-0.5</v>
       </c>
       <c r="O37" s="29">
-        <v>-7.6999999999999999E-2</v>
+        <v>0.58299999999999996</v>
       </c>
       <c r="P37" s="29">
-        <v>0.4</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="Q37" s="29">
-        <v>6.7000000000000004E-2</v>
+        <v>0.28199999999999997</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
@@ -4829,19 +4939,19 @@
         <v>33</v>
       </c>
       <c r="B38" s="30">
-        <v>1.429</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="C38" s="30">
-        <v>1.667</v>
+        <v>0.125</v>
       </c>
       <c r="D38" s="30">
-        <v>1.714</v>
+        <v>-0.25</v>
       </c>
       <c r="E38" s="30">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="F38" s="30">
-        <v>-1</v>
+        <v>-0.5</v>
+      </c>
+      <c r="F38" s="30" t="s">
+        <v>24</v>
       </c>
       <c r="G38" s="30" t="s">
         <v>24</v>
@@ -4850,31 +4960,31 @@
         <v>24</v>
       </c>
       <c r="I38" s="30">
-        <v>0.65400000000000003</v>
+        <v>-0.10100000000000001</v>
       </c>
       <c r="J38" s="30">
-        <v>1</v>
+        <v>-0.65400000000000003</v>
       </c>
       <c r="K38" s="30">
-        <v>0.27300000000000002</v>
+        <v>0.53600000000000003</v>
       </c>
       <c r="L38" s="30">
-        <v>0.54800000000000004</v>
+        <v>-0.20300000000000001</v>
       </c>
       <c r="M38" s="30">
-        <v>-0.20899999999999999</v>
+        <v>0.38200000000000001</v>
       </c>
       <c r="N38" s="30">
-        <v>3</v>
+        <v>-0.41699999999999998</v>
       </c>
       <c r="O38" s="30">
-        <v>1.5</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="P38" s="30">
-        <v>2.1760000000000002</v>
+        <v>-0.29599999999999999</v>
       </c>
       <c r="Q38" s="30">
-        <v>0.68899999999999995</v>
+        <v>-0.114</v>
       </c>
       <c r="T38" t="s">
         <v>25</v>
@@ -4887,50 +4997,50 @@
       <c r="B39" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C39" s="29" t="s">
-        <v>24</v>
+      <c r="C39" s="29">
+        <v>-1</v>
       </c>
       <c r="D39" s="29">
+        <v>1</v>
+      </c>
+      <c r="E39" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G39" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="I39" s="29">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="J39" s="29">
+        <v>-0.4</v>
+      </c>
+      <c r="K39" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="L39" s="29">
+        <v>0.25</v>
+      </c>
+      <c r="M39" s="29">
+        <v>2</v>
+      </c>
+      <c r="N39" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="O39" s="29">
         <v>-0.5</v>
       </c>
-      <c r="E39" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="F39" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="G39" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="H39" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I39" s="29">
-        <v>0.13400000000000001</v>
-      </c>
-      <c r="J39" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="K39" s="29">
-        <v>-1</v>
-      </c>
-      <c r="L39" s="29">
-        <v>0.111</v>
-      </c>
-      <c r="M39" s="29">
-        <v>-0.54500000000000004</v>
-      </c>
-      <c r="N39" s="29">
-        <v>-0.66700000000000004</v>
-      </c>
-      <c r="O39" s="29" t="s">
-        <v>24</v>
-      </c>
       <c r="P39" s="29">
-        <v>-0.66700000000000004</v>
+        <v>3</v>
       </c>
       <c r="Q39" s="29">
-        <v>0.10199999999999999</v>
+        <v>0.20799999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
@@ -4938,52 +5048,52 @@
         <v>35</v>
       </c>
       <c r="B40" s="30">
-        <v>0.5</v>
+        <v>-0.222</v>
       </c>
       <c r="C40" s="30">
-        <v>-0.25</v>
+        <v>0.111</v>
       </c>
       <c r="D40" s="30">
-        <v>0.68200000000000005</v>
+        <v>-0.45900000000000002</v>
       </c>
       <c r="E40" s="30">
-        <v>-0.125</v>
-      </c>
-      <c r="F40" s="30">
-        <v>-0.5</v>
+        <v>-0.14299999999999999</v>
+      </c>
+      <c r="F40" s="30" t="s">
+        <v>24</v>
       </c>
       <c r="G40" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="H40" s="30" t="s">
-        <v>24</v>
+      <c r="H40" s="30">
+        <v>1</v>
       </c>
       <c r="I40" s="30">
-        <v>-0.14799999999999999</v>
+        <v>0.36599999999999999</v>
       </c>
       <c r="J40" s="30">
-        <v>-0.15</v>
+        <v>0.64700000000000002</v>
       </c>
       <c r="K40" s="30">
-        <v>0.23100000000000001</v>
+        <v>0.313</v>
       </c>
       <c r="L40" s="30">
-        <v>-0.23499999999999999</v>
+        <v>0.56899999999999995</v>
       </c>
       <c r="M40" s="30">
-        <v>-1.7999999999999999E-2</v>
-      </c>
-      <c r="N40" s="30">
-        <v>0.42899999999999999</v>
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="N40" s="30" t="s">
+        <v>24</v>
       </c>
       <c r="O40" s="30">
-        <v>1.667</v>
+        <v>-7.4999999999999997E-2</v>
       </c>
       <c r="P40" s="30">
-        <v>0.622</v>
+        <v>0.3</v>
       </c>
       <c r="Q40" s="30">
-        <v>-7.8E-2</v>
+        <v>0.33100000000000002</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
@@ -4996,8 +5106,8 @@
       <c r="C41" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="29" t="s">
-        <v>24</v>
+      <c r="D41" s="29">
+        <v>1</v>
       </c>
       <c r="E41" s="29" t="s">
         <v>24</v>
@@ -5012,7 +5122,7 @@
         <v>24</v>
       </c>
       <c r="I41" s="29">
-        <v>-0.22800000000000001</v>
+        <v>0.51300000000000001</v>
       </c>
       <c r="J41" s="29" t="s">
         <v>24</v>
@@ -5021,22 +5131,22 @@
         <v>24</v>
       </c>
       <c r="L41" s="29">
-        <v>-0.38500000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="M41" s="29">
-        <v>-0.111</v>
+        <v>-0.125</v>
       </c>
       <c r="N41" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="O41" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="P41" s="29">
-        <v>-0.5</v>
+      <c r="O41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="P41" s="29" t="s">
+        <v>24</v>
       </c>
       <c r="Q41" s="29">
-        <v>-0.20300000000000001</v>
+        <v>0.45500000000000002</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
@@ -5049,35 +5159,35 @@
       <c r="C42" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D42" s="30">
+      <c r="D42" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G42" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I42" s="30">
+        <v>0.31</v>
+      </c>
+      <c r="J42" s="30">
         <v>-1</v>
       </c>
-      <c r="E42" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="F42" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="G42" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="H42" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="I42" s="30">
-        <v>-0.53200000000000003</v>
-      </c>
-      <c r="J42" s="30" t="s">
-        <v>24</v>
-      </c>
       <c r="K42" s="30" t="s">
         <v>24</v>
       </c>
       <c r="L42" s="30">
-        <v>0.25</v>
+        <v>-0.4</v>
       </c>
       <c r="M42" s="30">
-        <v>0.5</v>
+        <v>-0.33300000000000002</v>
       </c>
       <c r="N42" s="30" t="s">
         <v>24</v>
@@ -5085,11 +5195,11 @@
       <c r="O42" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="P42" s="30" t="s">
-        <v>24</v>
+      <c r="P42" s="30">
+        <v>-1</v>
       </c>
       <c r="Q42" s="30">
-        <v>-0.437</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
@@ -5099,156 +5209,156 @@
       <c r="B43" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C43" s="29" t="s">
-        <v>24</v>
+      <c r="C43" s="29">
+        <v>-0.33300000000000002</v>
       </c>
       <c r="D43" s="29">
-        <v>1.5</v>
+        <v>-0.2</v>
       </c>
       <c r="E43" s="29">
-        <v>-0.14299999999999999</v>
+        <v>-0.83299999999999996</v>
       </c>
       <c r="F43" s="29">
-        <v>-0.5</v>
-      </c>
-      <c r="G43" s="29" t="s">
-        <v>24</v>
+        <v>-1</v>
+      </c>
+      <c r="G43" s="29">
+        <v>-1</v>
       </c>
       <c r="H43" s="29" t="s">
         <v>24</v>
       </c>
       <c r="I43" s="29">
-        <v>0.27900000000000003</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="J43" s="29">
-        <v>4.625</v>
+        <v>-0.42199999999999999</v>
       </c>
       <c r="K43" s="29">
-        <v>0.5</v>
+        <v>-0.66700000000000004</v>
       </c>
       <c r="L43" s="29">
-        <v>-0.17100000000000001</v>
+        <v>1.5289999999999999</v>
       </c>
       <c r="M43" s="29">
-        <v>-0.13900000000000001</v>
-      </c>
-      <c r="N43" s="29">
-        <v>-1</v>
+        <v>-0.32300000000000001</v>
+      </c>
+      <c r="N43" s="29" t="s">
+        <v>24</v>
       </c>
       <c r="O43" s="29">
-        <v>-0.77800000000000002</v>
+        <v>3.5</v>
       </c>
       <c r="P43" s="29">
-        <v>-0.36799999999999999</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="Q43" s="29">
-        <v>0.24099999999999999</v>
+        <v>0.26300000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="30" t="s">
-        <v>24</v>
+      <c r="B44" s="30">
+        <v>-1</v>
       </c>
       <c r="C44" s="30">
-        <v>1</v>
-      </c>
-      <c r="D44" s="30">
+        <v>-0.5</v>
+      </c>
+      <c r="D44" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="30">
         <v>-1</v>
       </c>
-      <c r="E44" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="F44" s="30">
-        <v>-0.77800000000000002</v>
+      <c r="F44" s="30" t="s">
+        <v>24</v>
       </c>
       <c r="G44" s="30">
-        <v>-0.88900000000000001</v>
+        <v>-1</v>
       </c>
       <c r="H44" s="30" t="s">
         <v>24</v>
       </c>
       <c r="I44" s="30">
-        <v>1.333</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="J44" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="K44" s="30" t="s">
-        <v>24</v>
+      <c r="K44" s="30">
+        <v>-1</v>
       </c>
       <c r="L44" s="30">
-        <v>-0.69199999999999995</v>
+        <v>1.25</v>
       </c>
       <c r="M44" s="30">
-        <v>-0.83299999999999996</v>
-      </c>
-      <c r="N44" s="30">
-        <v>-1</v>
-      </c>
-      <c r="O44" s="30">
-        <v>-1</v>
+        <v>2</v>
+      </c>
+      <c r="N44" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="O44" s="30" t="s">
+        <v>24</v>
       </c>
       <c r="P44" s="30" t="s">
         <v>24</v>
       </c>
       <c r="Q44" s="30">
-        <v>-0.55400000000000005</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B45" s="29">
-        <v>1</v>
+      <c r="B45" s="29" t="s">
+        <v>24</v>
       </c>
       <c r="C45" s="29">
-        <v>3</v>
+        <v>-0.5</v>
       </c>
       <c r="D45" s="29">
-        <v>-0.71399999999999997</v>
+        <v>0.5</v>
       </c>
       <c r="E45" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="F45" s="29">
+      <c r="F45" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G45" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="H45" s="29">
         <v>-1</v>
       </c>
-      <c r="G45" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="H45" s="29" t="s">
-        <v>24</v>
-      </c>
       <c r="I45" s="29">
-        <v>-3.7999999999999999E-2</v>
-      </c>
-      <c r="J45" s="29">
-        <v>-0.5</v>
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="J45" s="29" t="s">
+        <v>24</v>
       </c>
       <c r="K45" s="29" t="s">
         <v>24</v>
       </c>
       <c r="L45" s="29">
-        <v>-0.42399999999999999</v>
+        <v>0.94699999999999995</v>
       </c>
       <c r="M45" s="29">
-        <v>1.75</v>
+        <v>-0.36399999999999999</v>
       </c>
       <c r="N45" s="29" t="s">
         <v>24</v>
       </c>
       <c r="O45" s="29">
-        <v>4</v>
+        <v>-0.2</v>
       </c>
       <c r="P45" s="29">
-        <v>-0.5</v>
+        <v>1</v>
       </c>
       <c r="Q45" s="29">
-        <v>-5.8999999999999997E-2</v>
+        <v>0.17199999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
@@ -5259,19 +5369,19 @@
         <v>24</v>
       </c>
       <c r="C46" s="30">
-        <v>-0.5</v>
+        <v>0.6</v>
       </c>
       <c r="D46" s="30">
-        <v>0.4</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E46" s="30">
-        <v>-0.5</v>
+        <v>3</v>
       </c>
       <c r="F46" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="G46" s="30">
-        <v>-1</v>
+      <c r="G46" s="30" t="s">
+        <v>24</v>
       </c>
       <c r="H46" s="30" t="s">
         <v>24</v>
@@ -5280,28 +5390,28 @@
         <v>0.115</v>
       </c>
       <c r="J46" s="30">
-        <v>-0.88900000000000001</v>
+        <v>1</v>
       </c>
       <c r="K46" s="30">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="L46" s="30">
-        <v>0.28999999999999998</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="M46" s="30">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="N46" s="30" t="s">
-        <v>24</v>
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="N46" s="30">
+        <v>6</v>
       </c>
       <c r="O46" s="30">
-        <v>-0.66700000000000004</v>
-      </c>
-      <c r="P46" s="30">
-        <v>0.16700000000000001</v>
+        <v>13</v>
+      </c>
+      <c r="P46" s="30" t="s">
+        <v>24</v>
       </c>
       <c r="Q46" s="30">
-        <v>8.6999999999999994E-2</v>
+        <v>0.214</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
@@ -5309,16 +5419,16 @@
         <v>42</v>
       </c>
       <c r="B47" s="29">
-        <v>2.6669999999999998</v>
-      </c>
-      <c r="C47" s="29">
-        <v>-1</v>
+        <v>-0.36399999999999999</v>
+      </c>
+      <c r="C47" s="29" t="s">
+        <v>24</v>
       </c>
       <c r="D47" s="29">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="E47" s="29">
-        <v>1</v>
+        <v>-0.16700000000000001</v>
       </c>
       <c r="F47" s="29" t="s">
         <v>24</v>
@@ -5326,35 +5436,35 @@
       <c r="G47" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="H47" s="29" t="s">
-        <v>24</v>
+      <c r="H47" s="29">
+        <v>1</v>
       </c>
       <c r="I47" s="29">
-        <v>0.29299999999999998</v>
+        <v>0.41499999999999998</v>
       </c>
       <c r="J47" s="29">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="K47" s="29">
-        <v>1.8</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="L47" s="29">
-        <v>0.125</v>
+        <v>0.88900000000000001</v>
       </c>
       <c r="M47" s="29">
-        <v>0.125</v>
-      </c>
-      <c r="N47" s="29">
-        <v>-1</v>
+        <v>-0.33300000000000002</v>
+      </c>
+      <c r="N47" s="29" t="s">
+        <v>24</v>
       </c>
       <c r="O47" s="29">
-        <v>-0.28599999999999998</v>
+        <v>-0.2</v>
       </c>
       <c r="P47" s="29">
-        <v>2</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="Q47" s="29">
-        <v>0.372</v>
+        <v>0.28799999999999998</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
@@ -5364,11 +5474,11 @@
       <c r="B48" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C48" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D48" s="30" t="s">
-        <v>24</v>
+      <c r="C48" s="30">
+        <v>-1</v>
+      </c>
+      <c r="D48" s="30">
+        <v>4</v>
       </c>
       <c r="E48" s="30" t="s">
         <v>24</v>
@@ -5383,137 +5493,137 @@
         <v>24</v>
       </c>
       <c r="I48" s="30">
-        <v>-0.10100000000000001</v>
-      </c>
-      <c r="J48" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="K48" s="30" t="s">
-        <v>24</v>
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="J48" s="30">
+        <v>2</v>
+      </c>
+      <c r="K48" s="30">
+        <v>-0.5</v>
       </c>
       <c r="L48" s="30">
-        <v>-8.3000000000000004E-2</v>
+        <v>0.182</v>
       </c>
       <c r="M48" s="30">
-        <v>-0.375</v>
-      </c>
-      <c r="N48" s="30" t="s">
-        <v>24</v>
+        <v>1.4</v>
+      </c>
+      <c r="N48" s="30">
+        <v>-1</v>
       </c>
       <c r="O48" s="30" t="s">
         <v>24</v>
       </c>
       <c r="P48" s="30">
-        <v>-0.5</v>
+        <v>4</v>
       </c>
       <c r="Q48" s="30">
-        <v>-9.9000000000000005E-2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="29" t="s">
-        <v>24</v>
+      <c r="B49" s="29">
+        <v>-0.5</v>
       </c>
       <c r="C49" s="29">
-        <v>-0.16700000000000001</v>
+        <v>-0.2</v>
       </c>
       <c r="D49" s="29">
-        <v>0.182</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="E49" s="29">
-        <v>-0.25</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="F49" s="29">
-        <v>-0.5</v>
+        <v>6</v>
       </c>
       <c r="G49" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="H49" s="29">
-        <v>-1</v>
+      <c r="H49" s="29" t="s">
+        <v>24</v>
       </c>
       <c r="I49" s="29">
-        <v>-5.3999999999999999E-2</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="J49" s="29">
-        <v>-0.35</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="K49" s="29">
-        <v>-0.4</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="L49" s="29">
-        <v>-9.9000000000000005E-2</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="M49" s="29">
-        <v>-6.4000000000000001E-2</v>
-      </c>
-      <c r="N49" s="29">
-        <v>-0.16700000000000001</v>
-      </c>
-      <c r="O49" s="29">
-        <v>-0.29399999999999998</v>
+        <v>-2.3E-2</v>
+      </c>
+      <c r="N49" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="O49" s="29" t="s">
+        <v>24</v>
       </c>
       <c r="P49" s="29">
-        <v>-0.48099999999999998</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="Q49" s="29">
-        <v>-9.7000000000000003E-2</v>
+        <v>0.17599999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B50" s="30">
-        <v>0.66700000000000004</v>
+      <c r="B50" s="30" t="s">
+        <v>24</v>
       </c>
       <c r="C50" s="30" t="s">
         <v>24</v>
       </c>
       <c r="D50" s="30">
-        <v>-0.75</v>
+        <v>2</v>
       </c>
       <c r="E50" s="30">
+        <v>-1</v>
+      </c>
+      <c r="F50" s="30">
+        <v>-1</v>
+      </c>
+      <c r="G50" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="H50" s="30">
         <v>-0.5</v>
       </c>
-      <c r="F50" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="G50" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="H50" s="30" t="s">
-        <v>24</v>
-      </c>
       <c r="I50" s="30">
-        <v>-0.245</v>
+        <v>0.3</v>
       </c>
       <c r="J50" s="30">
-        <v>-0.44400000000000001</v>
-      </c>
-      <c r="K50" s="30" t="s">
-        <v>24</v>
+        <v>0.4</v>
+      </c>
+      <c r="K50" s="30">
+        <v>0.42899999999999999</v>
       </c>
       <c r="L50" s="30">
-        <v>-3.2000000000000001E-2</v>
-      </c>
-      <c r="M50" s="30" t="s">
-        <v>24</v>
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="M50" s="30">
+        <v>0.75</v>
       </c>
       <c r="N50" s="30">
-        <v>0.25</v>
+        <v>0.8</v>
       </c>
       <c r="O50" s="30">
-        <v>2</v>
+        <v>-0.55600000000000005</v>
       </c>
       <c r="P50" s="30">
-        <v>0.33300000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="Q50" s="30">
-        <v>-0.16900000000000001</v>
+        <v>0.308</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
@@ -5524,34 +5634,34 @@
         <v>24</v>
       </c>
       <c r="C51" s="29">
-        <v>-0.5</v>
-      </c>
-      <c r="D51" s="29">
         <v>-1</v>
       </c>
+      <c r="D51" s="29" t="s">
+        <v>24</v>
+      </c>
       <c r="E51" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="F51" s="29">
-        <v>-0.88900000000000001</v>
-      </c>
-      <c r="G51" s="29">
+      <c r="F51" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G51" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="H51" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="I51" s="29">
+        <v>0.2</v>
+      </c>
+      <c r="J51" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="K51" s="29">
         <v>-1</v>
       </c>
-      <c r="H51" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I51" s="29">
-        <v>-0.28599999999999998</v>
-      </c>
-      <c r="J51" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="K51" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="L51" s="29" t="s">
-        <v>24</v>
+      <c r="L51" s="29">
+        <v>2</v>
       </c>
       <c r="M51" s="29" t="s">
         <v>24</v>
@@ -5566,60 +5676,60 @@
         <v>24</v>
       </c>
       <c r="Q51" s="29">
-        <v>-0.59099999999999997</v>
+        <v>0.44400000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C52" s="30">
+      <c r="B52" s="30">
         <v>-1</v>
       </c>
+      <c r="C52" s="30" t="s">
+        <v>24</v>
+      </c>
       <c r="D52" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E52" s="30">
+      <c r="E52" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F52" s="30">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="G52" s="30">
         <v>-1</v>
       </c>
-      <c r="F52" s="30">
-        <v>2</v>
-      </c>
-      <c r="G52" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="H52" s="30" t="s">
-        <v>24</v>
+      <c r="H52" s="30">
+        <v>-1</v>
       </c>
       <c r="I52" s="30">
-        <v>-0.14099999999999999</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="J52" s="30">
-        <v>2</v>
-      </c>
-      <c r="K52" s="30">
-        <v>-1</v>
+        <v>1</v>
+      </c>
+      <c r="K52" s="30" t="s">
+        <v>24</v>
       </c>
       <c r="L52" s="30">
-        <v>-0.45500000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="M52" s="30">
-        <v>-0.47099999999999997</v>
+        <v>0.77800000000000002</v>
       </c>
       <c r="N52" s="30">
-        <v>-0.4</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="O52" s="30">
-        <v>2.5</v>
+        <v>-0.42899999999999999</v>
       </c>
       <c r="P52" s="30">
-        <v>0.16700000000000001</v>
+        <v>-0.28599999999999998</v>
       </c>
       <c r="Q52" s="30">
-        <v>-0.158</v>
+        <v>0.115</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
@@ -5627,60 +5737,60 @@
         <v>18</v>
       </c>
       <c r="B53" s="29">
-        <v>1</v>
+        <v>-0.76900000000000002</v>
       </c>
       <c r="C53" s="29">
-        <v>-0.61199999999999999</v>
+        <v>-0.52600000000000002</v>
       </c>
       <c r="D53" s="29">
-        <v>-0.34200000000000003</v>
+        <v>-0.68799999999999994</v>
       </c>
       <c r="E53" s="29">
-        <v>-0.57099999999999995</v>
+        <v>-0.66700000000000004</v>
       </c>
       <c r="F53" s="29">
-        <v>-0.63600000000000001</v>
+        <v>-0.75</v>
       </c>
       <c r="G53" s="29">
-        <v>-0.85699999999999998</v>
+        <v>1</v>
       </c>
       <c r="H53" s="29">
-        <v>-0.25</v>
+        <v>-0.33300000000000002</v>
       </c>
       <c r="I53" s="29">
-        <v>-0.34100000000000003</v>
+        <v>-0.52</v>
       </c>
       <c r="J53" s="29">
-        <v>-0.308</v>
+        <v>-0.47199999999999998</v>
       </c>
       <c r="K53" s="29">
-        <v>-0.16700000000000001</v>
+        <v>-0.629</v>
       </c>
       <c r="L53" s="29">
-        <v>-0.35299999999999998</v>
+        <v>-0.624</v>
       </c>
       <c r="M53" s="29">
-        <v>-0.313</v>
+        <v>-0.51500000000000001</v>
       </c>
       <c r="N53" s="29">
-        <v>7.6999999999999999E-2</v>
+        <v>-0.64300000000000002</v>
       </c>
       <c r="O53" s="29">
-        <v>4.2000000000000003E-2</v>
+        <v>-0.70299999999999996</v>
       </c>
       <c r="P53" s="29">
-        <v>-0.29399999999999998</v>
+        <v>-0.20799999999999999</v>
       </c>
       <c r="Q53" s="29">
-        <v>-0.33200000000000002</v>
+        <v>-0.53800000000000003</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B54" s="30" t="s">
-        <v>24</v>
+      <c r="B54" s="30">
+        <v>-1</v>
       </c>
       <c r="C54" s="30" t="s">
         <v>24</v>
@@ -5701,31 +5811,31 @@
         <v>24</v>
       </c>
       <c r="I54" s="30">
-        <v>-4.2000000000000003E-2</v>
+        <v>-0.435</v>
       </c>
       <c r="J54" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="K54" s="30">
-        <v>-1</v>
+      <c r="K54" s="30" t="s">
+        <v>24</v>
       </c>
       <c r="L54" s="30">
-        <v>-0.25</v>
+        <v>-0.66700000000000004</v>
       </c>
       <c r="M54" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="N54" s="30">
-        <v>-1</v>
-      </c>
-      <c r="O54" s="30">
-        <v>-1</v>
+      <c r="N54" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="O54" s="30" t="s">
+        <v>24</v>
       </c>
       <c r="P54" s="30">
-        <v>3</v>
+        <v>-0.5</v>
       </c>
       <c r="Q54" s="30">
-        <v>-8.7999999999999995E-2</v>
+        <v>-0.41899999999999998</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>